<commit_message>
Added basic code for outputing links to named references
</commit_message>
<xml_diff>
--- a/examples/getsetranges.xlsx
+++ b/examples/getsetranges.xlsx
@@ -9,6 +9,13 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="A">Sheet1!$B$1</definedName>
+    <definedName name="B">Sheet1!$B$2</definedName>
+    <definedName name="C_">Sheet1!$B$3</definedName>
+    <definedName name="range">Sheet1!$B$1:$B$3</definedName>
+    <definedName name="Total">Sheet1!$B$4</definedName>
+  </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -402,7 +409,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -436,7 +443,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <f>SUM(B1:B3)</f>
+        <f>SUM(range)</f>
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed a bug when named references are specified as well as cells to keep and named reference points to blanks
</commit_message>
<xml_diff>
--- a/examples/getsetranges.xlsx
+++ b/examples/getsetranges.xlsx
@@ -14,6 +14,7 @@
     <definedName name="B">Sheet1!$B$2</definedName>
     <definedName name="C_">Sheet1!$B$3</definedName>
     <definedName name="range">Sheet1!$B$1:$B$3</definedName>
+    <definedName name="RangeOverBlanks">Sheet1!$B$6:$F$6</definedName>
     <definedName name="Total">Sheet1!$B$4</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>A</t>
   </si>
@@ -38,6 +39,9 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>RangeOverBlanks</t>
   </si>
 </sst>
 </file>
@@ -406,15 +410,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -422,7 +426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -430,7 +434,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -438,13 +442,30 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
         <f>SUM(range)</f>
         <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <f>B1</f>
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <f>B2</f>
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <f>B3</f>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>